<commit_message>
Save 1 frame on PPW-2
</commit_message>
<xml_diff>
--- a/rayman_saxPercentTas_times.xlsx
+++ b/rayman_saxPercentTas_times.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fuerchter\Downloads\BizHawk-1.10.0\Movies\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="24915" windowHeight="12330"/>
   </bookViews>
@@ -207,7 +202,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -223,9 +218,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -263,9 +258,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -300,7 +295,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -335,7 +330,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -512,11 +507,11 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A2:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="1.7109375" customWidth="1"/>
@@ -647,7 +642,7 @@
         <v>5714</v>
       </c>
       <c r="E8" s="1">
-        <v>7541</v>
+        <v>7540</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -665,7 +660,9 @@
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1">
+        <v>7543</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1162,7 +1159,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1175,7 +1172,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
PPW-B (b for bad)
</commit_message>
<xml_diff>
--- a/rayman_saxPercentTas_times.xlsx
+++ b/rayman_saxPercentTas_times.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fuerchter\Downloads\BizHawk-1.10.0\Movies\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="24915" windowHeight="12330"/>
   </bookViews>
@@ -202,7 +207,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -218,9 +223,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -258,9 +263,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -295,7 +300,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -330,7 +335,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -507,11 +512,11 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A2:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="1.7109375" customWidth="1"/>
@@ -663,7 +668,9 @@
       <c r="D9" s="1">
         <v>7543</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1">
+        <v>9206</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1159,7 +1166,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1172,7 +1179,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
The correct bk2 for sax% (accidentially pushed an empty movie earlier) Updated the splits (but unsure on how to write down the lag frames)
</commit_message>
<xml_diff>
--- a/rayman_saxPercentTas_times.xlsx
+++ b/rayman_saxPercentTas_times.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fuerchter\Downloads\BizHawk-1.11.0\Movies\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="24915" windowHeight="12330"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t xml:space="preserve">Rayman </t>
   </si>
@@ -139,6 +144,12 @@
   </si>
   <si>
     <t>Timesheet</t>
+  </si>
+  <si>
+    <t>+2 from end on</t>
+  </si>
+  <si>
+    <t>+3</t>
   </si>
 </sst>
 </file>
@@ -182,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -200,9 +211,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -218,9 +232,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -258,9 +272,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -295,7 +309,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -330,7 +344,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -507,11 +521,11 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A2:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="1.7109375" customWidth="1"/>
@@ -617,16 +631,18 @@
         <v>4</v>
       </c>
       <c r="D7" s="1">
-        <v>4629</v>
+        <v>4632</v>
       </c>
       <c r="E7" s="1">
-        <v>5713</v>
+        <v>5716</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
+      <c r="K7" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
@@ -639,10 +655,10 @@
         <v>5</v>
       </c>
       <c r="D8" s="1">
-        <v>5714</v>
+        <v>5717</v>
       </c>
       <c r="E8" s="1">
-        <v>7540</v>
+        <v>7543</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -661,10 +677,10 @@
         <v>6</v>
       </c>
       <c r="D9" s="1">
-        <v>7543</v>
+        <v>7546</v>
       </c>
       <c r="E9" s="1">
-        <v>9181</v>
+        <v>9200</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -686,7 +702,7 @@
         <v>9201</v>
       </c>
       <c r="E10" s="1">
-        <v>10893</v>
+        <v>10895</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1">
@@ -694,7 +710,9 @@
       </c>
       <c r="H10" s="1"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
+      <c r="K10" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
@@ -725,10 +743,10 @@
         <v>14</v>
       </c>
       <c r="D12" s="1">
-        <v>11467</v>
+        <v>11469</v>
       </c>
       <c r="E12" s="1">
-        <v>12975</v>
+        <v>12977</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -747,10 +765,10 @@
         <v>15</v>
       </c>
       <c r="D13" s="1">
-        <v>12976</v>
+        <v>12978</v>
       </c>
       <c r="E13" s="1">
-        <v>15805</v>
+        <v>15807</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -769,10 +787,10 @@
         <v>16</v>
       </c>
       <c r="D14" s="1">
-        <v>15809</v>
+        <v>15811</v>
       </c>
       <c r="E14" s="1">
-        <v>19451</v>
+        <v>19453</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1">
@@ -793,10 +811,10 @@
         <v>17</v>
       </c>
       <c r="D15" s="1">
-        <v>19454</v>
+        <v>19456</v>
       </c>
       <c r="E15" s="1">
-        <v>20806</v>
+        <v>20808</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1">
@@ -835,7 +853,7 @@
         <v>20</v>
       </c>
       <c r="D17" s="1">
-        <v>21717</v>
+        <v>21719</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1189,7 +1207,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1202,7 +1220,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
sax%: progress! (still need to update the spreadsheet)
</commit_message>
<xml_diff>
--- a/rayman_saxPercentTas_times.xlsx
+++ b/rayman_saxPercentTas_times.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fuerchter\Downloads\BizHawk-1.11.0\Movies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fuerchter2\Downloads\BizHawk-1.11.0\Movies\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="24915" windowHeight="12330"/>
+    <workbookView xWindow="120" yWindow="96" windowWidth="24912" windowHeight="12336"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t xml:space="preserve">Rayman </t>
   </si>
@@ -56,9 +56,6 @@
     <t>End Frame</t>
   </si>
   <si>
-    <t>Lag</t>
-  </si>
-  <si>
     <t>End</t>
   </si>
   <si>
@@ -146,10 +143,7 @@
     <t>Timesheet</t>
   </si>
   <si>
-    <t>+2 from end on</t>
-  </si>
-  <si>
-    <t>+3</t>
+    <t>Lag Counter</t>
   </si>
 </sst>
 </file>
@@ -208,11 +202,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -522,20 +516,20 @@
   <dimension ref="A2:Q36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="1.7109375" customWidth="1"/>
-    <col min="3" max="5" width="11.42578125" style="3"/>
-    <col min="6" max="6" width="0.85546875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="3"/>
-    <col min="9" max="9" width="0.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="1.6640625" customWidth="1"/>
+    <col min="3" max="5" width="11.44140625" style="3"/>
+    <col min="6" max="6" width="0.88671875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" style="3"/>
+    <col min="9" max="9" width="0.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
@@ -543,11 +537,11 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L2" s="5"/>
       <c r="N2" s="5"/>
@@ -555,7 +549,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
@@ -565,15 +559,15 @@
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D4" s="6" t="s">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="D4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="G4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="6"/>
+      <c r="E4" s="7"/>
+      <c r="G4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="7"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
@@ -583,9 +577,9 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C5" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>9</v>
@@ -597,7 +591,7 @@
         <v>8</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
@@ -608,7 +602,7 @@
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -626,7 +620,7 @@
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
@@ -640,9 +634,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="K7" s="6"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
@@ -650,7 +642,7 @@
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
     </row>
-    <row r="8" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
@@ -672,7 +664,7 @@
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
@@ -694,7 +686,7 @@
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
     </row>
-    <row r="10" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C10" s="3" t="s">
         <v>7</v>
       </c>
@@ -706,13 +698,11 @@
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1">
-        <v>989</v>
+        <v>986</v>
       </c>
       <c r="H10" s="1"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="K10" s="6"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
@@ -720,9 +710,9 @@
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
     </row>
-    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -738,9 +728,9 @@
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
     </row>
-    <row r="12" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C12" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" s="1">
         <v>11469</v>
@@ -760,9 +750,9 @@
       <c r="P12" s="5"/>
       <c r="Q12" s="5"/>
     </row>
-    <row r="13" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C13" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" s="1">
         <v>12978</v>
@@ -782,9 +772,9 @@
       <c r="P13" s="5"/>
       <c r="Q13" s="5"/>
     </row>
-    <row r="14" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C14" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D14" s="1">
         <v>15811</v>
@@ -794,7 +784,7 @@
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1">
-        <v>1003</v>
+        <v>999</v>
       </c>
       <c r="H14" s="1"/>
       <c r="J14" s="5"/>
@@ -806,9 +796,9 @@
       <c r="P14" s="5"/>
       <c r="Q14" s="5"/>
     </row>
-    <row r="15" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C15" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D15" s="1">
         <v>19456</v>
@@ -818,7 +808,7 @@
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1">
-        <v>1005</v>
+        <v>1002</v>
       </c>
       <c r="H15" s="1"/>
       <c r="J15" s="5"/>
@@ -830,9 +820,9 @@
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
     </row>
-    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -848,9 +838,9 @@
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
     </row>
-    <row r="17" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="1">
         <v>21719</v>
@@ -868,9 +858,9 @@
       <c r="P17" s="5"/>
       <c r="Q17" s="5"/>
     </row>
-    <row r="18" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C18" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -886,9 +876,9 @@
       <c r="P18" s="5"/>
       <c r="Q18" s="5"/>
     </row>
-    <row r="19" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C19" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -904,9 +894,9 @@
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
     </row>
-    <row r="20" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -922,9 +912,9 @@
       <c r="P20" s="5"/>
       <c r="Q20" s="5"/>
     </row>
-    <row r="21" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C21" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -940,9 +930,9 @@
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
     </row>
-    <row r="22" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C22" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -958,9 +948,9 @@
       <c r="P22" s="5"/>
       <c r="Q22" s="5"/>
     </row>
-    <row r="23" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -976,9 +966,9 @@
       <c r="P23" s="5"/>
       <c r="Q23" s="5"/>
     </row>
-    <row r="24" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C24" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -994,9 +984,9 @@
       <c r="P24" s="5"/>
       <c r="Q24" s="5"/>
     </row>
-    <row r="25" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C25" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -1012,9 +1002,9 @@
       <c r="P25" s="5"/>
       <c r="Q25" s="5"/>
     </row>
-    <row r="26" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C26" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1030,9 +1020,9 @@
       <c r="P26" s="5"/>
       <c r="Q26" s="5"/>
     </row>
-    <row r="27" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C27" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1048,9 +1038,9 @@
       <c r="P27" s="5"/>
       <c r="Q27" s="5"/>
     </row>
-    <row r="28" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C28" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -1066,9 +1056,9 @@
       <c r="P28" s="5"/>
       <c r="Q28" s="5"/>
     </row>
-    <row r="29" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1084,9 +1074,9 @@
       <c r="P29" s="5"/>
       <c r="Q29" s="5"/>
     </row>
-    <row r="30" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C30" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -1102,9 +1092,9 @@
       <c r="P30" s="5"/>
       <c r="Q30" s="5"/>
     </row>
-    <row r="31" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C31" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -1120,9 +1110,9 @@
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
     </row>
-    <row r="32" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1138,9 +1128,9 @@
       <c r="P32" s="5"/>
       <c r="Q32" s="5"/>
     </row>
-    <row r="33" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C33" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -1156,9 +1146,9 @@
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
     </row>
-    <row r="34" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C34" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1168,9 +1158,9 @@
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
     </row>
-    <row r="35" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" outlineLevel="1" x14ac:dyDescent="0.3">
       <c r="C35" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -1180,9 +1170,9 @@
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -1207,7 +1197,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1220,7 +1210,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
sax% - BH-4, BH-5
</commit_message>
<xml_diff>
--- a/rayman_saxPercentTas_times.xlsx
+++ b/rayman_saxPercentTas_times.xlsx
@@ -515,8 +515,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A2:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -845,7 +845,9 @@
       <c r="D17" s="1">
         <v>21719</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="1">
+        <v>23314</v>
+      </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -862,8 +864,12 @@
       <c r="C18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="D18" s="1">
+        <v>23315</v>
+      </c>
+      <c r="E18" s="1">
+        <v>25879</v>
+      </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -880,8 +886,12 @@
       <c r="C19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="D19" s="1">
+        <v>25880</v>
+      </c>
+      <c r="E19" s="1">
+        <v>27836</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -898,8 +908,12 @@
       <c r="C20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="D20" s="1">
+        <v>27837</v>
+      </c>
+      <c r="E20" s="1">
+        <v>31212</v>
+      </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -916,8 +930,12 @@
       <c r="C21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="D21" s="1">
+        <v>31213</v>
+      </c>
+      <c r="E21" s="1">
+        <v>34713</v>
+      </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -934,7 +952,9 @@
       <c r="C22" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="1"/>
+      <c r="D22" s="1">
+        <v>34714</v>
+      </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>

</xml_diff>

<commit_message>
sax% - Finished Bongo Hills for now
</commit_message>
<xml_diff>
--- a/rayman_saxPercentTas_times.xlsx
+++ b/rayman_saxPercentTas_times.xlsx
@@ -516,7 +516,7 @@
   <dimension ref="A2:Q36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -955,7 +955,9 @@
       <c r="D22" s="1">
         <v>34714</v>
       </c>
-      <c r="E22" s="1"/>
+      <c r="E22" s="1">
+        <v>37087</v>
+      </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -990,7 +992,9 @@
       <c r="C24" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="1"/>
+      <c r="D24" s="1">
+        <v>37631</v>
+      </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>

</xml_diff>

<commit_message>
sax% - AP-1 and 2
</commit_message>
<xml_diff>
--- a/rayman_saxPercentTas_times.xlsx
+++ b/rayman_saxPercentTas_times.xlsx
@@ -516,7 +516,7 @@
   <dimension ref="A2:Q36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -995,7 +995,9 @@
       <c r="D24" s="1">
         <v>37631</v>
       </c>
-      <c r="E24" s="1"/>
+      <c r="E24" s="1">
+        <v>38698</v>
+      </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -1012,8 +1014,12 @@
       <c r="C25" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="D25" s="1">
+        <v>38699</v>
+      </c>
+      <c r="E25" s="1">
+        <v>40702</v>
+      </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -1030,7 +1036,9 @@
       <c r="C26" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="1"/>
+      <c r="D26" s="1">
+        <v>40703</v>
+      </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>

</xml_diff>